<commit_message>
error corrected in isnumber feature
</commit_message>
<xml_diff>
--- a/contents.xlsx
+++ b/contents.xlsx
@@ -436,12 +436,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> අඩවි ගොඩක් හින්දියෙන් කතා කරන්න යන්නේ ඔයාගේ computer එක කොහොමද automatically shutdown කරන්න කියලා අපි හිතුවා මොකද file එකක් download වෙන්න දාල දෙනවා එහෙම නැත්තං වෙන්නේ දාලා තියෙනවා වෙන්න දාලා තියෙනවා එතකොට පැය දානකම් පෙර ගෙඩියක් බලන් ඉන්න ඕනේ කීයට හරි මේක shutdown කරන්න අපිට ඕන වෙලාවක් දාලා මේක shutdown automatically software නැතුව කරගන්න පුළුවන් ඒක අපිට ගොඩක් ලොකු පහසුවක් වෙයි බලන්න මීට කලින් කරමු windows tips බලන්න චනුක්ස් windows 10 අමතක කරන්න එපා මේකට වර කිසිම සොෆ්ට්වෙයා ඕනෙ නැහැ ඔන්න බලන්න ඔයාගේ computer එකේ ස්ටාර්ට් එකට ගිහිල්ලා මේ රන් කියන එකට යන්න ගියාට පස්සේ මට මෙන්න මේ විදියේ කත් බලාගන්න පුළුවන් මෙතන ඔයාට හරිම කෙටියෙන් shutdown space minus a space minus කියලා ගහලා කොච්චර වෙලාවකින් the shutdown වෙන්න ඕනේ කියලා තත්පර වලින් ගහන්න මෙතන හැට ගහන එකෙන් මට විනාඩියකින් තප්පර 60කින් තමයි shutdown වෙන්න ඕනෙ නම් මෙතෙන්ට කරපු ගමන් s ගියාට පස්සෙ automatically මේ විදියට වගේ computer එක shutdown වෙනවා කොයි තරං ලේසි ද ඔයා මෙතනින් 60 ගහන්නේ විනාඩියකින් sundown වෙන්න කියන්න 120 කියන්නේ විනාඩි දෙකකින් shutdown වෙන්න කියන්න 1818 මෙන්න මෙතන 3610 පුළුවන් වැද්දෝ නං ඔයාට මෙතන 7200 ටයිප් කරන්න පුළුවන් මං හිතන්නේ මේක ගොඩක් use ටිප් එකක් ඒ වගේම කොහොමද ටයිප් කරන්න ඕනේ නැහැ පුංචි icon එකක් එකට දාගන්න පුලුවන් නම් මේක කරලා පෙන්වමු මට තේරුම් ගන්න පුළුවන් වෙයි පුළුවන් වෙබ් එකේ ෆොටෝ එකක් ඇතුලෙ write creative short cuts ඔන්න ඊට පස්සේ අර කලින් කියපු command එක මෙතන ටයිප් කරන්න තමයි තියෙන්නේ මම මේ විදිහට shutdown s t හැටයි කියල විනාඩියකින් වෙන්න දාලා නෙක්ස්ට් කරන්න පස්සෙ ඔයාට ආයි ගහනවා මං මේක ශබ්ද කියලම දිලා next කරන්න පසුවට පෙන්න ඇති icon එකක් ආවා ඔයාට ඕනෙනම් එක මෙහෙම පාවිච්චි කරන්න පුළුවන් නැත්තං ඒක right click කරල properties සිංහල වන කැමති icon එකක් දාගන්නත් පුළුවන් ඔයාට මේක පැයකින් හරි ඔයා ටයිප් කරන්න ඕනම වෙලාවක කෝල් කරලා ගියපු ගමන් automatically shutdown වෙනවා අද අපි කතා කරපු simple php එක නොහිතන මේ දවස් වල from home ගෙදර ඉඳන් venizuela කරනවා ඒ වගේම ගෙදර ඉඳන් පාඩම් කරනවා එතකොට පරිගණකේ මේ පුංචි පුංචි පුංචි අපිට නිතරම පාවිච්චි කරන්න පුළුවන් මේක ගොඩක් use කරගන්න අපිට හොඳ කෝල් එකක් වෙනවා ඒ වගේම මට මේ minus ඒ වෙනුවට mina සර් කියලා ගැහුවොත් computer එකක් වට අවශ්‍ය වෙලාවක දීමේ ස්ටාර්ට් කරගන්නත් පුළුවන් එකාට මොන ට්‍රිප් එකක් නෙමෙයි දේවල් බලන්න subscribe කරන්න instu game එකෙක් එපා කරන්න යාලුවෙක්ට දැනගන්න මේ වීඩියෝ එක ශෙයා කරන්න උදව් සිංහයෙකුගෙන් අලුත් දෙවල් ගොඩක් මට හමුවෙමු</t>
+          <t xml:space="preserve"> මගේ තියෙන සැම්සුන්ග් ගැලැක්සි ෆෝන් එකක් ආසන්න වශයෙන් රුපියල් දෙලක්ෂ හැත්තෑ දාහකට විතර තමයි මිළදීගත ඉගෙන ලක්ෂ තුනක් විතර මේ ඉතිං එකේ value එක මේ ෆෝන් එක රුපියල් පනස්දාහට විතර බස්සන්න පුළුවන් වුණා මෙන්න මේ පුංචි එක නිසා අඩු වෙනුවෙන් ඉගෙන ගන්න යන්නේ වගේ ස්මාට් ෆෝන් එකේ screen එක අනිවාර්යෙන්ම කන වගේ රැක ගන්න වෙනවා එහෙම නැත්නම් මගේ ෆෝන් එකේ value එක විතර නැති වෙන්න ඕන තරම් ඉඩ තියෙනවා මේකෙ මෙන්න මේ වගේ පුංචි දූ එකක් තමයි වෙන්නේ ආවෙ ඇත්තම මේ ස්ක්‍රීන් එක රීප්ලේස් කරන්න රුපියල් කීයක් යනවා කියලද ඔයාල හිතාගෙන ඉන්නේ මම ඒක ඔයාට කියනවට වැඩිය අපි samsung service center එකට කතා කරල බලමු සැම්සුං ගැලැක්සි නෝට්ටුව bro ෆෝන් එකේ screen එක රීප්ලේස් කරන්න රුපියල් කීයක් යනවද කියලා ක්‍රීම් එක රීප්ලේස් කරන්න වෙන අවස්ථා මොනවද ඔයා things when එක හිතෙන්න පුළුවන් ඔයාගෙන් ෆෝන් එක වැටෙන්න පුළුවන් ඔයා thing පෝන් එක ප්‍රෙස් වෙන්න පුළුවන් විශේෂම ෆෝන් එක සාක්කුවේ දාගෙන ඉන්නකොට ෆෝන් එකක් හද වෙන්න පුළුවන් වෙන මේ වගේ අවස්ථා ගණනාවකදී මේ ස්ක්‍රීන් එක සම්පූර්ණයෙන්ම ඩැමේජ් ජල යන්න ඕන තරම් ඉඩ තියෙනවා අපි gorillaz නෙමෙයි මොන තරම් strength එකක් තියෙන මොනතරම් song ග්ලාස් එකක් මේකට දාල තිබුනත් රහස් කැඩෙනවා glass බිඳෙනවා මේවා හානි වෙනවා කියන එක හොයාගෙන ගන්න ඕනේ නෑනේ කරල අපි හිතමු මේක රුපියල් දෙලක්ෂ හැත්තෑ දාකට අපි මිලදී ගත්තා එතකොට මේකේ second hand market එක මේ වෙනකොට තියෙන්නේ ගෙන මාස හයකට විතර පස්සෙ 150000 190000 විතරක් අතර පිරින් එතකොට අපි වේගය murders case එක ගත්තොත් screen එකක් වට දාන් ආසන්න වශයෙන් රුපියල් ලක්ෂයක් විතර යනවා නේ අමු දෙදහස් කියන්නේ ඉතින් ඊට පස්සේ ඔයාට මේක විකුණන්න සිද්ධවෙන්නේ එකේ value එක වෙනුවෙන් රුපියල් පනස් දාහක් විතර තමයි මම එක රීප්ලේස් කරන්න ගියාම ඒ ගොල්ල කියන්නේ මේක දැන් පක්ෂවලට හොඳයි මේ පුංචි ඉතින් ඒ screen එකේ value එක එහෙමද touch screen එකේ මිල ගණන් මෙච්චර වැඩි නිසා තමයි ෆෝන් එකේ value එක මේ විදියට වේගයෙන් අඩු වෙන්න පටන් අරගෙන තියෙන්නේ තමයි මම පොඩ්ඩක් නෙට් එකේ සර්ච් කරලා බැලුවා ඉන්ටර්නෙට් එකෙන් එකක්නෙ place කරන්න රුපියල් කීයක් යනවද කියලා ඇතිනේ ඩොලර් 269 කියලා තමයි දෙක ආසන්න වශයෙන් රුපියල් දෙදහක් විතර ax1 එතකොට service charge හරි මොනාහරි 92000 ඇත්තටම ටිකක් ලොකු ගානක් ඉගෙන ගන්න තියෙන පාඩම තමයි අපි screen එක ගොඩක් හොඳට රැකගන්න නම් අර කලින් කියපු විදිහට වෙන්න ගත්තා ලේසියෙන්ම ඩැමේජ් වෙන්න ඉඩ තියෙනවා අපි හිතන්නෙවත් නැති වෙලාවේ ගොඩක් වෙලාවට hemi use කරන්නැති පෝන් එකක් වුණත් මේ විදිහට ස්ප්‍රින් එක tamil වෙන්න ඕන තරම් ඉඩ තියෙනවා මං හිතන්නේ කරමින් සිටින්නේ ගෙන ආ වගේ ෆෝන් එකේ screen එක ඩැමේජ් වෙලා තියෙනවද කොච්චර කාලෙකට කලින් ද ඒ වගේම මොකක් කරන්න ගියාද screen එක එයි දිනේ එක රීප්ලේස් කරන්න රුපියල් කීයද ෆෝන් එක මොකක්ද වගේ දේවල් අපි පොඩ්ඩක් පලයන් මේ සාකච්ඡා කරමු ඔයාගේ ඒ කමෙන්ට් ටික එකතු කරලා අපිට තව වීඩියෝ එකක් හදන්න පුළුවන් වෙයි ශ්‍රී ලංකාවේ මේය ස්මාට් ෆෝන් වල ස්ක්‍රීන් භාවිතය ගැන ඉතින් අවසාන වශයෙන් අපි ඉගෙන ගන්න තියෙන පාඩම තමයි ෆෝන් එකක් මිලදී ගන්න කොට අපි screen protector එකක් පාවිච්චි කරන්න ඕනේ ඒ වගේම බැක් කවර් එකක් වගේ දෙයක් පාවිච්චි කරන්න ද මේකෙ front එකේ එඩ්‍රස් එක වගේ වෙනවා ඇම්බැක්කේ ගියාම අපිට ඒ වගේම ටිකක් ලොකු මුදලක් එක රීප්ලේස් කරන්න එන නිසා ෆෝන් එකටත් ඇක්ෂන් එකක් දාගන්න සිද්ධ වෙනවා කියලා තමයි අද වීඩියෝ එක අද වීඩියෝ ගැන මට හිතුන දේවල් අනිවාර්යෙන් පල කෑම කන්න ගෙන් දන්නවාට තව ගැටලු තියෙනවනම් palagama සෙක්ස් උන්ගෙන් අපි සාකච්ඡා කරමු ඊලගට අපි බලමු මේක රිප්ලේස් කරන්න ගියාම මේකට උන්ට කිරීම කරන්න පුළුවන් වෙයිද ඒ මං ගත්තම ඒකට අපිට මුදල් ගෙවන්නේ වෙයිද එක රීප්ලේස් කරන්න රුපියල් කීයක් යයිද එතකොට කොච්චර දින ගණනක් යයිද මේ හැමදෙයක්ම අපි වෙනුවෙන් කතා කරන්න බලාපොරොත්තු වෙනවා කරන්න install කරන්න යාලුවෙක් දැන ගන්න වීඩියෝ එක ශෙයා කරන්න ඉගෙන සිංහල ගීක් ෂෝ එකේ අලුත් දේවල් ගොඩක් කරන්න හම්බ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2wbfT7ciNBs</t>
+          <t>yZD3oerZ_Pw</t>
         </is>
       </c>
     </row>

</xml_diff>